<commit_message>
implementet class panel 5 and corrected meta data for reference
</commit_message>
<xml_diff>
--- a/Data/Data_description_main.xlsx
+++ b/Data/Data_description_main.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\OneDrive\Data_Science\Sem2_Application_Project\MoinCC-AI4metabolomics\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93BE0DBF-EB2F-4393-AD6B-0C3BDA2D8955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86179E4F-CFD6-4282-95B9-0454D7F09760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1244,8 +1244,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C78" sqref="C78"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G72" sqref="G72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6231,9 +6231,7 @@
       <c r="I69" s="9">
         <v>11</v>
       </c>
-      <c r="J69" s="10">
-        <v>4.7</v>
-      </c>
+      <c r="J69" s="10"/>
       <c r="K69" s="8"/>
       <c r="L69" s="8"/>
       <c r="M69" s="11">
@@ -6427,9 +6425,7 @@
         <v>1</v>
       </c>
       <c r="I72" s="9"/>
-      <c r="J72" s="10">
-        <v>4.7</v>
-      </c>
+      <c r="J72" s="10"/>
       <c r="K72" s="8"/>
       <c r="L72" s="8"/>
       <c r="M72" s="11">

</xml_diff>